<commit_message>
debugged, and plot the graph of 5 spheres
</commit_message>
<xml_diff>
--- a/data/Washed_DD_T2_Five_Spheres_All_in_One.xlsx
+++ b/data/Washed_DD_T2_Five_Spheres_All_in_One.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinhanmei/Desktop/LME-and-CME-Essay/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DABD27-E800-1046-BA7A-2F2E70B3FB49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD90721-6A2D-7D49-8A64-4267C4A44B3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collective Bargaining Coverage" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="50">
   <si>
     <t>Year</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Austria</t>
-  </si>
-  <si>
-    <t>..</t>
   </si>
   <si>
     <t>Australia</t>
@@ -184,10 +181,6 @@
     <t>Country Name</t>
   </si>
   <si>
-    <t>..</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Canada</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -262,12 +255,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -572,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
@@ -647,27 +643,12 @@
       <c r="G2">
         <v>98</v>
       </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
       <c r="J2">
         <v>98</v>
       </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
       <c r="L2">
         <v>98</v>
       </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
       <c r="O2">
         <v>98</v>
       </c>
@@ -686,66 +667,39 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
       <c r="D3">
         <v>58.8</v>
       </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3">
         <v>59.3</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="H3">
         <v>59.4</v>
       </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
       <c r="J3">
         <v>54.9</v>
       </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
       <c r="L3">
         <v>58.7</v>
       </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
       <c r="N3">
         <v>58.1</v>
       </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
       <c r="P3">
         <v>60.1</v>
       </c>
-      <c r="Q3" t="s">
-        <v>20</v>
-      </c>
       <c r="R3">
         <v>60</v>
       </c>
-      <c r="S3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>96</v>
@@ -804,7 +758,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>30.4</v>
@@ -863,7 +817,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>77.7</v>
@@ -919,32 +873,20 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>85</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7">
         <v>91</v>
       </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
       <c r="F7">
         <v>91.4</v>
       </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
       <c r="H7">
         <v>87.7</v>
       </c>
-      <c r="I7" t="s">
-        <v>20</v>
-      </c>
       <c r="J7">
         <v>84.7</v>
       </c>
@@ -954,28 +896,19 @@
       <c r="L7">
         <v>77.8</v>
       </c>
-      <c r="M7" t="s">
-        <v>20</v>
-      </c>
       <c r="N7">
         <v>89.7</v>
       </c>
-      <c r="O7" t="s">
-        <v>20</v>
-      </c>
       <c r="P7">
         <v>89.3</v>
       </c>
       <c r="Q7">
         <v>89.3</v>
       </c>
-      <c r="R7" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>67.8</v>
@@ -1031,7 +964,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>44.2</v>
@@ -1039,31 +972,16 @@
       <c r="G9">
         <v>41.7</v>
       </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" t="s">
-        <v>20</v>
-      </c>
       <c r="K9">
         <v>40.5</v>
       </c>
       <c r="P9">
         <v>32.5</v>
       </c>
-      <c r="Q9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>21.1</v>
@@ -1110,7 +1028,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>81.7</v>
@@ -1169,19 +1087,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F12">
         <v>74.5</v>
@@ -1189,24 +1095,9 @@
       <c r="G12">
         <v>74.2</v>
       </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" t="s">
-        <v>20</v>
-      </c>
       <c r="J12">
         <v>73.5</v>
       </c>
-      <c r="K12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" t="s">
-        <v>20</v>
-      </c>
       <c r="N12">
         <v>73.099999999999994</v>
       </c>
@@ -1216,16 +1107,10 @@
       <c r="P12">
         <v>72.5</v>
       </c>
-      <c r="Q12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R12" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>20</v>
@@ -1239,71 +1124,29 @@
       <c r="E13">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
       <c r="I13">
         <v>17.8</v>
       </c>
-      <c r="J13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" t="s">
-        <v>20</v>
-      </c>
       <c r="L13">
         <v>15.6</v>
       </c>
       <c r="M13">
         <v>15.3</v>
       </c>
-      <c r="N13" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>94</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
       <c r="D14">
         <v>94</v>
       </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
       <c r="G14">
         <v>93</v>
       </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
       <c r="I14">
         <v>89.5</v>
       </c>
@@ -1337,44 +1180,26 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>39.9</v>
       </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
       <c r="E15">
         <v>41.8</v>
       </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
       <c r="G15">
         <v>44.6</v>
       </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
       <c r="I15">
         <v>44.8</v>
       </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
       <c r="K15">
         <v>44.9</v>
       </c>
       <c r="L15">
         <v>54.2</v>
       </c>
-      <c r="M15" t="s">
-        <v>20</v>
-      </c>
       <c r="N15">
         <v>57.3</v>
       </c>
@@ -1384,16 +1209,13 @@
       <c r="P15">
         <v>57.1</v>
       </c>
-      <c r="Q15" t="s">
-        <v>20</v>
-      </c>
       <c r="R15">
         <v>57.9</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>36.4</v>
@@ -1452,7 +1274,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>14.2</v>
@@ -1511,20 +1333,11 @@
     </row>
     <row r="18" spans="1:19">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18">
         <v>96.1</v>
       </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
       <c r="J18">
         <v>98</v>
       </c>
@@ -1534,31 +1347,16 @@
       <c r="L18">
         <v>98</v>
       </c>
-      <c r="M18" t="s">
-        <v>20</v>
-      </c>
       <c r="N18">
         <v>98</v>
       </c>
-      <c r="O18" t="s">
-        <v>20</v>
-      </c>
       <c r="P18">
         <v>98.5</v>
       </c>
-      <c r="Q18" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18" t="s">
-        <v>20</v>
-      </c>
-      <c r="S18" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>100</v>
@@ -1614,7 +1412,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>80</v>
@@ -1625,28 +1423,19 @@
       <c r="L20">
         <v>80</v>
       </c>
-      <c r="M20" t="s">
-        <v>20</v>
-      </c>
       <c r="N20">
         <v>80</v>
       </c>
-      <c r="O20" t="s">
-        <v>20</v>
-      </c>
       <c r="P20">
         <v>80</v>
       </c>
-      <c r="Q20" t="s">
-        <v>20</v>
-      </c>
       <c r="R20">
         <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>78.400000000000006</v>
@@ -1702,7 +1491,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>15.2</v>
@@ -1758,10 +1547,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>90.9</v>
@@ -1814,7 +1600,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>35.299999999999997</v>
@@ -1870,7 +1656,7 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>38.4</v>
@@ -1917,16 +1703,10 @@
       <c r="P25">
         <v>22.8</v>
       </c>
-      <c r="Q25" t="s">
-        <v>20</v>
-      </c>
-      <c r="R25" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="26" spans="1:19">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -1937,9 +1717,6 @@
       <c r="J26">
         <v>18.7</v>
       </c>
-      <c r="K26" t="s">
-        <v>20</v>
-      </c>
       <c r="L26">
         <v>18.600000000000001</v>
       </c>
@@ -1949,22 +1726,13 @@
       <c r="N26">
         <v>17.7</v>
       </c>
-      <c r="O26" t="s">
-        <v>20</v>
-      </c>
-      <c r="P26" t="s">
-        <v>20</v>
-      </c>
       <c r="Q26">
         <v>17.2</v>
       </c>
-      <c r="R26" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>12.6</v>
@@ -2036,7 +1804,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2093,7 +1861,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2148,7 +1916,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>76.703750999999997</v>
@@ -2210,7 +1978,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>75.092308000000003</v>
@@ -2272,7 +2040,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>75.989211999999995</v>
@@ -2334,7 +2102,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>80.931572000000003</v>
@@ -2396,7 +2164,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>75.15316</v>
@@ -2452,7 +2220,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>70.378203999999997</v>
@@ -2514,7 +2282,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>76.554810000000003</v>
@@ -2573,7 +2341,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>79.44117</v>
@@ -2635,7 +2403,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <v>82.418602000000007</v>
@@ -2682,7 +2450,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>80.01215400000001</v>
@@ -2744,7 +2512,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>81.662719999999993</v>
@@ -2806,7 +2574,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>81.430428000000006</v>
@@ -2868,7 +2636,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>81.101631000000012</v>
@@ -2930,7 +2698,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>76.681938000000002</v>
@@ -2992,7 +2760,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>75.211029000000011</v>
@@ -3054,7 +2822,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>64.586844999999997</v>
@@ -3116,7 +2884,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>71.228003999999999</v>
@@ -3178,7 +2946,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>83.253365000000002</v>
@@ -3240,7 +3008,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>68.740852000000004</v>
@@ -3302,7 +3070,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>71.992583999999994</v>
@@ -3364,7 +3132,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>75.545920999999993</v>
@@ -3426,7 +3194,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>72.110061999999999</v>
@@ -3488,7 +3256,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>66.600746000000001</v>
@@ -3550,7 +3318,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>64.027846999999994</v>
@@ -3628,7 +3396,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3685,7 +3453,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -3740,7 +3508,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>31.372516999999998</v>
@@ -3802,7 +3570,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>36.020634000000001</v>
@@ -3864,7 +3632,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>48.400092999999998</v>
@@ -3926,7 +3694,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>29.295521000000001</v>
@@ -3988,7 +3756,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>38.671585</v>
@@ -4044,7 +3812,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>22.250971</v>
@@ -4106,7 +3874,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>29.803612000000001</v>
@@ -4165,7 +3933,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>47.844825999999998</v>
@@ -4227,7 +3995,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>26.57077</v>
@@ -4289,7 +4057,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12">
         <v>40.902965999999999</v>
@@ -4336,7 +4104,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13">
         <v>40.402225000000001</v>
@@ -4356,7 +4124,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>33.639328000000013</v>
@@ -4418,7 +4186,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>25.571111999999999</v>
@@ -4480,7 +4248,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>28.901674</v>
@@ -4542,7 +4310,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>38.083973</v>
@@ -4604,7 +4372,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>31.375710999999999</v>
@@ -4666,7 +4434,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>23.921938000000001</v>
@@ -4728,7 +4496,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>10.429003</v>
@@ -4790,7 +4558,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>12.948861000000001</v>
@@ -4852,7 +4620,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>36.812420000000003</v>
@@ -4914,7 +4682,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>33.978282999999998</v>
@@ -4976,7 +4744,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>11.199056000000001</v>
@@ -5038,7 +4806,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>14.693064</v>
@@ -5100,7 +4868,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>14.184260999999999</v>
@@ -5162,7 +4930,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>8.8802375999999992</v>
@@ -5233,14 +5001,14 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:V1048576"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -5297,7 +5065,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -5364,7 +5132,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -5426,7 +5194,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -5488,7 +5256,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5550,7 +5318,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -5612,7 +5380,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -5674,7 +5442,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -5733,7 +5501,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -5795,7 +5563,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -5857,7 +5625,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -5919,7 +5687,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -5981,7 +5749,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -6040,7 +5808,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -6099,7 +5867,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -6158,7 +5926,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -6220,7 +5988,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -6282,7 +6050,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -6344,7 +6112,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -6406,7 +6174,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -6468,7 +6236,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -6530,7 +6298,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -6592,7 +6360,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -6654,7 +6422,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -6716,7 +6484,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -6778,7 +6546,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6840,7 +6608,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -6918,7 +6686,7 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -6975,7 +6743,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -7042,7 +6810,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7104,7 +6872,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -7166,7 +6934,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -7228,7 +6996,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -7290,7 +7058,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -7352,7 +7120,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -7411,7 +7179,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -7473,7 +7241,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -7535,7 +7303,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -7597,7 +7365,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -7659,7 +7427,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -7718,7 +7486,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -7777,7 +7545,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -7836,7 +7604,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -7898,7 +7666,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -7960,7 +7728,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -8022,7 +7790,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -8084,7 +7852,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -8146,7 +7914,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -8208,7 +7976,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -8270,7 +8038,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -8332,7 +8100,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -8394,7 +8162,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -8456,7 +8224,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -8518,7 +8286,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -8573,15 +8341,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W39" sqref="W39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -8638,25 +8406,16 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
       <c r="E2">
         <v>10.3270384880856</v>
       </c>
@@ -8711,26 +8470,14 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3">
         <v>22.602908002590802</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3">
         <v>23.446475195822401</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="H3">
         <v>22.132327939676301</v>
       </c>
@@ -8776,7 +8523,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>13.1548657180511</v>
@@ -8841,7 +8588,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>21.157038349997801</v>
@@ -8906,7 +8653,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>22.4083329625104</v>
@@ -8971,7 +8718,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>20.476490833101501</v>
@@ -9036,7 +8783,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>14.8371182824574</v>
@@ -9101,7 +8848,7 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>19.039497691806201</v>
@@ -9166,90 +8913,21 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I10">
         <v>11.6453686998862</v>
       </c>
-      <c r="J10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" t="s">
-        <v>20</v>
-      </c>
       <c r="N10">
         <v>10.7836561426782</v>
       </c>
-      <c r="O10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" t="s">
-        <v>20</v>
-      </c>
       <c r="S10">
         <v>10.618646519184001</v>
       </c>
-      <c r="T10" t="s">
-        <v>20</v>
-      </c>
-      <c r="U10" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H11">
         <v>8.4829228245957005</v>
@@ -9296,28 +8974,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I12">
         <v>20.597392230354799</v>
@@ -9361,58 +9018,7 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="S13">
         <v>23.769741766949</v>
@@ -9426,7 +9032,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>15.6995132025561</v>
@@ -9491,7 +9097,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>16.161241734046399</v>
@@ -9556,7 +9162,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>19.5884585457915</v>
@@ -9621,72 +9227,12 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17" t="s">
-        <v>20</v>
-      </c>
-      <c r="P17" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R17" t="s">
-        <v>20</v>
-      </c>
-      <c r="S17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T17" t="s">
-        <v>20</v>
-      </c>
-      <c r="U17" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>15.7302507898901</v>
@@ -9751,7 +9297,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>9.3416327385276592</v>
@@ -9759,12 +9305,6 @@
       <c r="C19">
         <v>6.5502601839844896</v>
       </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
       <c r="F19">
         <v>10.140308008989599</v>
       </c>
@@ -9816,7 +9356,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>10.510389026081601</v>
@@ -9881,7 +9421,7 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>13.3225331640636</v>
@@ -9946,72 +9486,12 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" t="s">
-        <v>20</v>
-      </c>
-      <c r="N22" t="s">
-        <v>20</v>
-      </c>
-      <c r="O22" t="s">
-        <v>20</v>
-      </c>
-      <c r="P22" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>20</v>
-      </c>
-      <c r="R22" t="s">
-        <v>20</v>
-      </c>
-      <c r="S22" t="s">
-        <v>20</v>
-      </c>
-      <c r="T22" t="s">
-        <v>20</v>
-      </c>
-      <c r="U22" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>21.060619453997301</v>
@@ -10076,10 +9556,7 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C24">
         <v>15.0861260475634</v>
@@ -10141,7 +9618,7 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>11.6291412183147</v>
@@ -10206,7 +9683,7 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>13.472438964192101</v>
@@ -10271,19 +9748,7 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F27">
         <v>12.887908872238601</v>
@@ -10345,14 +9810,14 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -10446,7 +9911,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>1.4166666000000001</v>
@@ -10493,7 +9958,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>1.8452381</v>
@@ -10540,7 +10005,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>0.92063492999999996</v>
@@ -10587,7 +10052,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>2.1349206000000001</v>
@@ -10634,7 +10099,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>2.3095238</v>
@@ -10681,7 +10146,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>2.6785714999999999</v>
@@ -10728,7 +10193,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>1.4365079000000001</v>
@@ -10775,7 +10240,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>1.7023809000000001</v>
@@ -10822,7 +10287,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>2.8849206000000001</v>
@@ -10869,7 +10334,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>2.3333333000000001</v>
@@ -10916,7 +10381,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>1.2428570999999999</v>
@@ -10963,7 +10428,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>2.6547618000000002</v>
@@ -11010,7 +10475,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>1.5952381</v>
@@ -11057,7 +10522,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>1.2619047000000001</v>
@@ -11104,7 +10569,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>0.25666665999999999</v>
@@ -11151,7 +10616,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>2.3412700000000002</v>
@@ -11198,7 +10663,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>2.8015873</v>
@@ -11245,7 +10710,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>2.7619047000000001</v>
@@ -11292,7 +10757,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>4.5833335000000002</v>
@@ -11339,7 +10804,7 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>2.3690476</v>
@@ -11386,7 +10851,7 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>2.3571428999999999</v>
@@ -11433,7 +10898,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>3.3055555999999999</v>
@@ -11480,7 +10945,7 @@
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>2.0039682000000001</v>
@@ -11527,7 +10992,7 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>2.2301587999999999</v>
@@ -11574,7 +11039,7 @@
     </row>
     <row r="27" spans="1:15">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>2.3928571000000001</v>
@@ -11630,74 +11095,74 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2001</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2002</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2003</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2004</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2005</v>
-      </c>
-      <c r="H1" s="1">
-        <v>2006</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2007</v>
-      </c>
-      <c r="J1" s="1">
-        <v>2008</v>
-      </c>
-      <c r="K1" s="1">
-        <v>2009</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2010</v>
-      </c>
-      <c r="M1" s="1">
-        <v>2011</v>
-      </c>
-      <c r="N1" s="1">
-        <v>2012</v>
-      </c>
-      <c r="O1" s="1">
-        <v>2013</v>
-      </c>
-      <c r="P1" s="1">
-        <v>2014</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>2015</v>
-      </c>
-      <c r="R1" s="1">
-        <v>2016</v>
-      </c>
-      <c r="S1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="T1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="U1" s="1">
-        <v>2019</v>
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -11767,7 +11232,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>1470</v>
@@ -11832,7 +11297,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>640</v>
@@ -11897,7 +11362,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>2862</v>
@@ -11962,7 +11427,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>697</v>
@@ -12027,7 +11492,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>3118</v>
@@ -12092,7 +11557,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>373</v>
@@ -12157,7 +11622,7 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>1824</v>
@@ -12222,7 +11687,7 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>1169</v>
@@ -12257,9 +11722,6 @@
       <c r="L10">
         <v>968</v>
       </c>
-      <c r="M10" t="s">
-        <v>50</v>
-      </c>
       <c r="N10">
         <v>836</v>
       </c>
@@ -12287,7 +11749,7 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>530</v>
@@ -12352,7 +11814,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>1087</v>
@@ -12417,7 +11879,7 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>854</v>
@@ -12482,7 +11944,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>5171</v>
@@ -12547,7 +12009,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>14114</v>
@@ -12612,7 +12074,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>2416</v>
@@ -12677,7 +12139,7 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>1141</v>
@@ -12742,7 +12204,7 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>293</v>
@@ -12807,7 +12269,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>361</v>
@@ -12872,7 +12334,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>1138</v>
@@ -12937,7 +12399,7 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>313</v>
@@ -12987,9 +12449,7 @@
       <c r="Q21">
         <v>201</v>
       </c>
-      <c r="R21" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="R21" s="2"/>
       <c r="S21">
         <v>182</v>
       </c>
@@ -13002,7 +12462,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>279</v>
@@ -13067,7 +12527,7 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>425</v>
@@ -13132,7 +12592,7 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>80</v>
@@ -13167,9 +12627,7 @@
       <c r="L24">
         <v>269</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="M24" s="2"/>
       <c r="N24">
         <v>320</v>
       </c>
@@ -13206,14 +12664,17 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="2" width="8.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -13270,7 +12731,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -13337,26 +12798,14 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3">
         <v>95.16</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
       <c r="F3">
         <v>95.67</v>
       </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
       <c r="H3">
         <v>93.27</v>
       </c>
@@ -13393,13 +12842,10 @@
       <c r="S3">
         <v>94.73</v>
       </c>
-      <c r="T3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>90.87</v>
@@ -13461,7 +12907,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>87.52</v>
@@ -13523,7 +12969,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>90.26</v>
@@ -13585,7 +13031,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>83.54</v>
@@ -13647,7 +13093,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>87.26</v>
@@ -13709,14 +13155,11 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>94.05</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
       <c r="D9">
         <v>94.66</v>
       </c>
@@ -13771,7 +13214,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>85.48</v>
@@ -13812,28 +13255,10 @@
       <c r="N10">
         <v>86.3</v>
       </c>
-      <c r="O10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10" t="s">
-        <v>20</v>
-      </c>
-      <c r="T10" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>86.34</v>
@@ -13895,7 +13320,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>90.7</v>
@@ -13957,7 +13382,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>84.76</v>
@@ -14019,7 +13444,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>88.46</v>
@@ -14081,7 +13506,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>93.04</v>
@@ -14143,69 +13568,21 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>95.98</v>
       </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
       <c r="G16">
         <v>95.79</v>
       </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" t="s">
-        <v>20</v>
-      </c>
-      <c r="O16" t="s">
-        <v>20</v>
-      </c>
-      <c r="P16" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>20</v>
-      </c>
-      <c r="R16" t="s">
-        <v>20</v>
-      </c>
       <c r="S16">
         <v>96.05</v>
       </c>
-      <c r="T16" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>84.56</v>
@@ -14267,7 +13644,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>86.53</v>
@@ -14329,7 +13706,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>89.89</v>
@@ -14391,7 +13768,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>80.069999999999993</v>
@@ -14453,19 +13830,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F21">
         <v>74.239999999999995</v>
@@ -14515,7 +13880,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>67.819999999999993</v>
@@ -14577,7 +13942,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>90.74</v>
@@ -14639,7 +14004,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>92.88</v>
@@ -14701,10 +14066,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>88.28</v>
@@ -14763,7 +14125,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26">
         <v>79.66</v>
@@ -14834,14 +14196,14 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -14898,7 +14260,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -14965,7 +14327,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>89.781798857007161</v>
@@ -15027,7 +14389,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>77.255299788904125</v>
@@ -15089,7 +14451,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>103.8456481144938</v>
@@ -15151,7 +14513,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>68.116166470736999</v>
@@ -15171,7 +14533,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>233.58700235997711</v>
@@ -15191,7 +14553,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>65.370464831657245</v>
@@ -15253,7 +14615,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>82.003028601084438</v>
@@ -15315,7 +14677,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>64.597628227624142</v>
@@ -15377,7 +14739,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>153.79214658622541</v>
@@ -15436,7 +14798,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>38.408882830762373</v>
@@ -15498,7 +14860,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>35.370674933035147</v>
@@ -15560,7 +14922,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>125.6379588380681</v>
@@ -15574,13 +14936,10 @@
       <c r="E14">
         <v>87.241666276441947</v>
       </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>291.23341241971332</v>
@@ -15642,7 +15001,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>155.44489774627141</v>
@@ -15674,7 +15033,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>147.35897315447701</v>
@@ -15736,7 +15095,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>106.19454910255411</v>
@@ -15798,7 +15157,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>62.230110680401232</v>
@@ -15857,7 +15216,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>67.174620585094203</v>
@@ -15889,7 +15248,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>51.289261831875677</v>
@@ -15951,7 +15310,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>30.49362691060206</v>
@@ -16013,7 +15372,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>84.476160402314719</v>
@@ -16075,7 +15434,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>15.80898650538184</v>
@@ -16107,7 +15466,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25">
         <v>19.21178472364609</v>
@@ -16163,7 +15522,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>18.197784024914601</v>
@@ -16225,7 +15584,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>25.537063407890649</v>
@@ -16296,7 +15655,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -16339,10 +15698,10 @@
         <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -16391,7 +15750,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>680.29317040000001</v>
@@ -16435,7 +15794,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>268.89078929999999</v>
@@ -16479,7 +15838,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>1732.632494</v>
@@ -16496,9 +15855,6 @@
       <c r="F5">
         <v>1406.9727009999999</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
       <c r="H5">
         <v>1829.853699</v>
       </c>
@@ -16523,7 +15879,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>259.02157410000001</v>
@@ -16567,7 +15923,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>183.39670430000001</v>
@@ -16611,7 +15967,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>1097.0627899999999</v>
@@ -16655,7 +16011,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>100.2787143</v>
@@ -16699,13 +16055,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>935.12789110000006</v>
@@ -16737,13 +16087,10 @@
       <c r="M10">
         <v>2288.468801</v>
       </c>
-      <c r="N10" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>350.76088979999997</v>
@@ -16787,7 +16134,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>368.05937460000001</v>
@@ -16831,7 +16178,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>60.19071417</v>
@@ -16875,7 +16222,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>572.69458059999999</v>
@@ -16919,7 +16266,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>351.76250420000002</v>
@@ -16963,7 +16310,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>2033.4814140000001</v>
@@ -17007,7 +16354,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>37402.906320000002</v>
@@ -17051,7 +16398,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>1079.592091</v>
@@ -17095,7 +16442,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>26.075935489999999</v>
@@ -17112,9 +16459,6 @@
       <c r="F19">
         <v>13.753907910000001</v>
       </c>
-      <c r="G19" t="s">
-        <v>20</v>
-      </c>
       <c r="H19">
         <v>17.347787690000001</v>
       </c>
@@ -17139,7 +16483,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>176.47085269999999</v>
@@ -17183,7 +16527,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>154.63157419999999</v>
@@ -17227,7 +16571,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>798.91761989999998</v>
@@ -17271,7 +16615,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>368.56287479999997</v>
@@ -17315,7 +16659,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>3.462624302</v>
@@ -17359,7 +16703,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>15.30373921</v>
@@ -17403,7 +16747,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>65.728615050000002</v>
@@ -17456,14 +16800,14 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -17569,7 +16913,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>0.92700000000000005</v>
@@ -17622,7 +16966,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>2.7349999999999999</v>
@@ -17675,7 +17019,7 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>0.67500000000000004</v>
@@ -17728,7 +17072,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -17781,7 +17125,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>2.1179999999999999</v>
@@ -17834,7 +17178,7 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>1.31</v>
@@ -17887,7 +17231,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0.83200000000000007</v>
@@ -17940,7 +17284,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>0.56000000000000005</v>
@@ -17993,7 +17337,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>1.383</v>
@@ -18046,7 +17390,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>0.44500000000000001</v>
@@ -18099,7 +17443,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>1.3009999999999999</v>
@@ -18152,7 +17496,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>1.31</v>
@@ -18205,7 +17549,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>0.50600000000000001</v>
@@ -18258,7 +17602,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>0.28999999999999998</v>
@@ -18311,7 +17655,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>0.22900000000000001</v>
@@ -18364,7 +17708,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>1.4139999999999999</v>
@@ -18417,7 +17761,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>0.58899999999999997</v>
@@ -18470,7 +17814,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>0.39400000000000002</v>
@@ -18523,7 +17867,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>0.626</v>
@@ -18576,7 +17920,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>7.400000000000001E-2</v>
@@ -18629,7 +17973,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>1.637</v>
@@ -18682,7 +18026,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>0.56700000000000006</v>
@@ -18735,7 +18079,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>0.68599999999999994</v>
@@ -18788,7 +18132,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>0.86499999999999999</v>
@@ -18838,7 +18182,7 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>6.0000000000000001E-3</v>
@@ -18900,14 +18244,14 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+      <selection activeCell="B1" sqref="B1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -18964,7 +18308,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -19019,7 +18363,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>82.878608999999997</v>
@@ -19081,7 +18425,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>85.308243000000004</v>
@@ -19143,7 +18487,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>82.643623000000005</v>
@@ -19205,7 +18549,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>88.410697999999996</v>
@@ -19267,7 +18611,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>84.385688999999999</v>
@@ -19323,7 +18667,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>83.401244999999989</v>
@@ -19385,7 +18729,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>87.528755000000004</v>
@@ -19444,7 +18788,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>79.043960999999996</v>
@@ -19506,7 +18850,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>86.283089000000004</v>
@@ -19568,7 +18912,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12">
         <v>88.826957999999991</v>
@@ -19615,7 +18959,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>82.212578000000008</v>
@@ -19677,7 +19021,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>86.682968000000002</v>
@@ -19739,7 +19083,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>90.403908000000001</v>
@@ -19801,7 +19145,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>87.755996999999994</v>
@@ -19863,7 +19207,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>85.012268000000006</v>
@@ -19925,7 +19269,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>83.199218999999999</v>
@@ -19987,7 +19331,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>80.910438999999997</v>
@@ -20049,7 +19393,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>81.389374000000004</v>
@@ -20111,7 +19455,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>90.606468000000007</v>
@@ -20173,7 +19517,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>75.420128000000005</v>
@@ -20235,7 +19579,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>79.702477000000002</v>
@@ -20297,7 +19641,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24">
         <v>86.837058999999996</v>
@@ -20359,7 +19703,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>82.432106000000005</v>
@@ -20421,7 +19765,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>84.540633999999997</v>
@@ -20483,7 +19827,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>78.475754000000009</v>

</xml_diff>